<commit_message>
update layout sheet for corne5x3
</commit_message>
<xml_diff>
--- a/keyboard-configurations/fwk-v1/layout.xlsx
+++ b/keyboard-configurations/fwk-v1/layout.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ibrahim\repos\ibrahimmkhalid\dotFiles\keyboard-configurations\fwk-v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ibrahim\dotFiles\keyboard-configurations\fwk-v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A853DED2-5AB7-4E97-9DEB-9C36EB9E1085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF881FF-02E4-44D1-A4B7-1E112AB7F34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="9" r:id="rId1"/>
+    <sheet name="corne3x5" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="181">
   <si>
     <t>,</t>
   </si>
@@ -485,6 +486,84 @@
   </si>
   <si>
     <t>NUM__</t>
+  </si>
+  <si>
+    <t>DEL_3</t>
+  </si>
+  <si>
+    <t>SPC_4</t>
+  </si>
+  <si>
+    <t>TAB_1</t>
+  </si>
+  <si>
+    <t>BSPC_2</t>
+  </si>
+  <si>
+    <t>RIGHT</t>
+  </si>
+  <si>
+    <t>_1</t>
+  </si>
+  <si>
+    <t>BACK</t>
+  </si>
+  <si>
+    <t>FWD</t>
+  </si>
+  <si>
+    <t>RLD</t>
+  </si>
+  <si>
+    <t>_0</t>
+  </si>
+  <si>
+    <t>_2</t>
+  </si>
+  <si>
+    <t>BTN1</t>
+  </si>
+  <si>
+    <t>BTN2</t>
+  </si>
+  <si>
+    <t>BTN3</t>
+  </si>
+  <si>
+    <t>_3</t>
+  </si>
+  <si>
+    <t>_4</t>
+  </si>
+  <si>
+    <t>A_GUI</t>
+  </si>
+  <si>
+    <t>S_ALT</t>
+  </si>
+  <si>
+    <t>D_CTL</t>
+  </si>
+  <si>
+    <t>F_SFT</t>
+  </si>
+  <si>
+    <t>J_SFT</t>
+  </si>
+  <si>
+    <t>K_CTL</t>
+  </si>
+  <si>
+    <t>L_ALT</t>
+  </si>
+  <si>
+    <t>;: _GUI</t>
+  </si>
+  <si>
+    <t>BOOT</t>
+  </si>
+  <si>
+    <t>MENU</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1377,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1412,6 +1491,20 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1771,20 +1864,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091B5B9F-AE75-4F8B-A9DD-E45051CA35D8}">
   <dimension ref="A1:AD42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38:I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="15" width="8.42578125" style="1" customWidth="1"/>
+    <col min="2" max="15" width="8.44140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="9" style="1" customWidth="1"/>
-    <col min="17" max="30" width="8.42578125" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="1"/>
+    <col min="17" max="30" width="8.44140625" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>130</v>
       </c>
@@ -1862,7 +1955,7 @@
       </c>
       <c r="AD1" s="32"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="33"/>
       <c r="B2" s="9" t="s">
         <v>30</v>
@@ -1942,7 +2035,7 @@
       </c>
       <c r="AD2" s="13"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="33"/>
       <c r="B3" s="9" t="s">
         <v>30</v>
@@ -2022,7 +2115,7 @@
       </c>
       <c r="AD3" s="13"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="33"/>
       <c r="B4" s="15" t="s">
         <v>30</v>
@@ -2102,7 +2195,7 @@
       </c>
       <c r="AD4" s="20"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
       <c r="B5" s="3" t="s">
         <v>56</v>
@@ -2146,7 +2239,7 @@
       <c r="AC5" s="4"/>
       <c r="AD5" s="8"/>
     </row>
-    <row r="6" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="33"/>
       <c r="B6" s="21"/>
       <c r="C6" s="22"/>
@@ -2186,7 +2279,7 @@
       <c r="AC6" s="22"/>
       <c r="AD6" s="25"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>132</v>
       </c>
@@ -2264,7 +2357,7 @@
       </c>
       <c r="AD7" s="8"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="33"/>
       <c r="B8" s="9" t="s">
         <v>30</v>
@@ -2344,7 +2437,7 @@
       </c>
       <c r="AD8" s="26"/>
     </row>
-    <row r="9" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="33"/>
       <c r="B9" s="9" t="s">
         <v>30</v>
@@ -2424,7 +2517,7 @@
       </c>
       <c r="AD9" s="13"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="33"/>
       <c r="B10" s="15" t="s">
         <v>30</v>
@@ -2504,7 +2597,7 @@
       </c>
       <c r="AD10" s="20"/>
     </row>
-    <row r="11" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
       <c r="B11" s="3" t="s">
         <v>30</v>
@@ -2548,7 +2641,7 @@
       <c r="AC11" s="4"/>
       <c r="AD11" s="8"/>
     </row>
-    <row r="12" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="33"/>
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
@@ -2588,7 +2681,7 @@
       <c r="AC12" s="22"/>
       <c r="AD12" s="25"/>
     </row>
-    <row r="13" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>128</v>
       </c>
@@ -2646,7 +2739,7 @@
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
     </row>
-    <row r="14" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
       <c r="B14" s="9" t="s">
         <v>30</v>
@@ -2706,7 +2799,7 @@
       <c r="AC14" s="6"/>
       <c r="AD14" s="6"/>
     </row>
-    <row r="15" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
       <c r="B15" s="9" t="s">
         <v>30</v>
@@ -2766,7 +2859,7 @@
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
     </row>
-    <row r="16" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="33"/>
       <c r="B16" s="15" t="s">
         <v>30</v>
@@ -2826,7 +2919,7 @@
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
     </row>
-    <row r="17" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
       <c r="B17" s="3" t="s">
         <v>56</v>
@@ -2870,7 +2963,7 @@
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
     </row>
-    <row r="18" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="33"/>
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
@@ -2910,7 +3003,7 @@
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
     </row>
-    <row r="19" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>129</v>
       </c>
@@ -2968,7 +3061,7 @@
       <c r="AC19" s="6"/>
       <c r="AD19" s="6"/>
     </row>
-    <row r="20" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="33"/>
       <c r="B20" s="9" t="s">
         <v>30</v>
@@ -3028,7 +3121,7 @@
       <c r="AC20" s="6"/>
       <c r="AD20" s="6"/>
     </row>
-    <row r="21" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
       <c r="B21" s="9" t="s">
         <v>30</v>
@@ -3088,7 +3181,7 @@
       <c r="AC21" s="6"/>
       <c r="AD21" s="6"/>
     </row>
-    <row r="22" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="33"/>
       <c r="B22" s="15" t="s">
         <v>30</v>
@@ -3148,7 +3241,7 @@
       <c r="AC22" s="6"/>
       <c r="AD22" s="6"/>
     </row>
-    <row r="23" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="33"/>
       <c r="B23" s="3" t="s">
         <v>56</v>
@@ -3192,7 +3285,7 @@
       <c r="AC23" s="6"/>
       <c r="AD23" s="6"/>
     </row>
-    <row r="24" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="33"/>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
@@ -3232,7 +3325,7 @@
       <c r="AC24" s="6"/>
       <c r="AD24" s="6"/>
     </row>
-    <row r="25" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>154</v>
       </c>
@@ -3290,7 +3383,7 @@
       <c r="AC25" s="6"/>
       <c r="AD25" s="6"/>
     </row>
-    <row r="26" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="33"/>
       <c r="B26" s="9" t="s">
         <v>30</v>
@@ -3350,7 +3443,7 @@
       <c r="AC26" s="6"/>
       <c r="AD26" s="6"/>
     </row>
-    <row r="27" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="33"/>
       <c r="B27" s="9" t="s">
         <v>30</v>
@@ -3410,7 +3503,7 @@
       <c r="AC27" s="6"/>
       <c r="AD27" s="6"/>
     </row>
-    <row r="28" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="33"/>
       <c r="B28" s="15" t="s">
         <v>30</v>
@@ -3470,7 +3563,7 @@
       <c r="AC28" s="6"/>
       <c r="AD28" s="6"/>
     </row>
-    <row r="29" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="33"/>
       <c r="B29" s="3" t="s">
         <v>56</v>
@@ -3514,7 +3607,7 @@
       <c r="AC29" s="6"/>
       <c r="AD29" s="6"/>
     </row>
-    <row r="30" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="34"/>
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
@@ -3554,7 +3647,7 @@
       <c r="AC30" s="6"/>
       <c r="AD30" s="6"/>
     </row>
-    <row r="31" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>143</v>
       </c>
@@ -3612,7 +3705,7 @@
       <c r="AC31" s="6"/>
       <c r="AD31" s="6"/>
     </row>
-    <row r="32" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="33"/>
       <c r="B32" s="9" t="s">
         <v>30</v>
@@ -3672,7 +3765,7 @@
       <c r="AC32" s="6"/>
       <c r="AD32" s="6"/>
     </row>
-    <row r="33" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="33"/>
       <c r="B33" s="9" t="s">
         <v>30</v>
@@ -3732,7 +3825,7 @@
       <c r="AC33" s="6"/>
       <c r="AD33" s="6"/>
     </row>
-    <row r="34" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="33"/>
       <c r="B34" s="15" t="s">
         <v>30</v>
@@ -3792,7 +3885,7 @@
       <c r="AC34" s="6"/>
       <c r="AD34" s="6"/>
     </row>
-    <row r="35" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="33"/>
       <c r="B35" s="3" t="s">
         <v>30</v>
@@ -3838,7 +3931,7 @@
       <c r="AC35" s="6"/>
       <c r="AD35" s="6"/>
     </row>
-    <row r="36" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="34"/>
       <c r="B36" s="21"/>
       <c r="C36" s="22"/>
@@ -3880,7 +3973,7 @@
       <c r="AC36" s="6"/>
       <c r="AD36" s="6"/>
     </row>
-    <row r="37" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>131</v>
       </c>
@@ -3923,7 +4016,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="33"/>
       <c r="B38" s="9" t="s">
         <v>58</v>
@@ -3968,7 +4061,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="33"/>
       <c r="B39" s="9" t="s">
         <v>60</v>
@@ -4013,7 +4106,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="33"/>
       <c r="B40" s="15" t="s">
         <v>47</v>
@@ -4058,7 +4151,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="33"/>
       <c r="B41" s="3" t="s">
         <v>56</v>
@@ -4087,7 +4180,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="38"/>
       <c r="B42" s="21"/>
       <c r="C42" s="22"/>
@@ -4116,4 +4209,1944 @@
   <pageMargins left="0.41" right="0" top="0.28299999999999997" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C4DEAC-AE2C-4CD8-9CB8-A21BA41D0651}">
+  <dimension ref="A1:AE42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="15" width="8.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9" style="1" customWidth="1"/>
+    <col min="17" max="30" width="8.44140625" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="44"/>
+    </row>
+    <row r="2" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="33"/>
+      <c r="B2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="44"/>
+    </row>
+    <row r="3" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="33"/>
+      <c r="B3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="43"/>
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="43"/>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="43"/>
+      <c r="AD3" s="43"/>
+      <c r="AE3" s="44"/>
+    </row>
+    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
+      <c r="B4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="43"/>
+      <c r="AE4" s="44"/>
+    </row>
+    <row r="5" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
+      <c r="B5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="43"/>
+      <c r="Y5" s="43"/>
+      <c r="Z5" s="43"/>
+      <c r="AA5" s="43"/>
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="43"/>
+      <c r="AD5" s="43"/>
+      <c r="AE5" s="44"/>
+    </row>
+    <row r="6" spans="1:31" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="33"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="N6" s="22"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="43"/>
+      <c r="X6" s="43"/>
+      <c r="Y6" s="43"/>
+      <c r="Z6" s="43"/>
+      <c r="AA6" s="43"/>
+      <c r="AB6" s="43"/>
+      <c r="AC6" s="43"/>
+      <c r="AD6" s="43"/>
+      <c r="AE6" s="44"/>
+    </row>
+    <row r="7" spans="1:31" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="43"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="43"/>
+      <c r="W7" s="43"/>
+      <c r="X7" s="43"/>
+      <c r="Y7" s="43"/>
+      <c r="Z7" s="43"/>
+      <c r="AA7" s="43"/>
+      <c r="AB7" s="43"/>
+      <c r="AC7" s="43"/>
+      <c r="AD7" s="43"/>
+      <c r="AE7" s="44"/>
+    </row>
+    <row r="8" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="33"/>
+      <c r="B8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="43"/>
+      <c r="X8" s="43"/>
+      <c r="Y8" s="43"/>
+      <c r="Z8" s="43"/>
+      <c r="AA8" s="43"/>
+      <c r="AB8" s="43"/>
+      <c r="AC8" s="43"/>
+      <c r="AD8" s="45"/>
+      <c r="AE8" s="44"/>
+    </row>
+    <row r="9" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="33"/>
+      <c r="B9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="43"/>
+      <c r="X9" s="43"/>
+      <c r="Y9" s="43"/>
+      <c r="Z9" s="43"/>
+      <c r="AA9" s="43"/>
+      <c r="AB9" s="43"/>
+      <c r="AC9" s="43"/>
+      <c r="AD9" s="43"/>
+      <c r="AE9" s="44"/>
+    </row>
+    <row r="10" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="43"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="43"/>
+      <c r="X10" s="43"/>
+      <c r="Y10" s="43"/>
+      <c r="Z10" s="43"/>
+      <c r="AA10" s="43"/>
+      <c r="AB10" s="43"/>
+      <c r="AC10" s="43"/>
+      <c r="AD10" s="43"/>
+      <c r="AE10" s="44"/>
+    </row>
+    <row r="11" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="33"/>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="43"/>
+      <c r="X11" s="43"/>
+      <c r="Y11" s="43"/>
+      <c r="Z11" s="43"/>
+      <c r="AA11" s="43"/>
+      <c r="AB11" s="43"/>
+      <c r="AC11" s="43"/>
+      <c r="AD11" s="43"/>
+      <c r="AE11" s="44"/>
+    </row>
+    <row r="12" spans="1:31" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="33"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="N12" s="22"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43"/>
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="43"/>
+      <c r="AD12" s="43"/>
+      <c r="AE12" s="44"/>
+    </row>
+    <row r="13" spans="1:31" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
+      <c r="U13" s="43"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="43"/>
+      <c r="X13" s="43"/>
+      <c r="Y13" s="43"/>
+      <c r="Z13" s="43"/>
+      <c r="AA13" s="43"/>
+      <c r="AB13" s="43"/>
+      <c r="AC13" s="43"/>
+      <c r="AD13" s="43"/>
+      <c r="AE13" s="44"/>
+    </row>
+    <row r="14" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="33"/>
+      <c r="B14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>2</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3</v>
+      </c>
+      <c r="F14" s="6">
+        <v>4</v>
+      </c>
+      <c r="G14" s="10">
+        <v>5</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="12">
+        <v>6</v>
+      </c>
+      <c r="K14" s="6">
+        <v>7</v>
+      </c>
+      <c r="L14" s="6">
+        <v>8</v>
+      </c>
+      <c r="M14" s="6">
+        <v>9</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0</v>
+      </c>
+      <c r="O14" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
+    </row>
+    <row r="15" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="33"/>
+      <c r="B15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+    </row>
+    <row r="16" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="33"/>
+      <c r="B16" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="N16" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="O16" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+    </row>
+    <row r="17" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="33"/>
+      <c r="B17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="O17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+    </row>
+    <row r="18" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="33"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" s="22"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6"/>
+    </row>
+    <row r="19" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="6"/>
+    </row>
+    <row r="20" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="33"/>
+      <c r="B20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O20" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+    </row>
+    <row r="21" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="33"/>
+      <c r="B21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="O21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6"/>
+    </row>
+    <row r="22" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="33"/>
+      <c r="B22" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="O22" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="6"/>
+    </row>
+    <row r="23" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="33"/>
+      <c r="B23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
+    </row>
+    <row r="24" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="33"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M24" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="N24" s="22"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="6"/>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6"/>
+    </row>
+    <row r="25" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="O25" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" s="35"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="6"/>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="6"/>
+    </row>
+    <row r="26" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="33"/>
+      <c r="B26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="M26" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="N26" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O26" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="6"/>
+    </row>
+    <row r="27" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="33"/>
+      <c r="B27" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="L27" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="M27" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="N27" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="6"/>
+    </row>
+    <row r="28" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="33"/>
+      <c r="B28" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="L28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="M28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="N28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="O28" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="6"/>
+    </row>
+    <row r="29" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="33"/>
+      <c r="B29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="6"/>
+      <c r="Z29" s="6"/>
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="6"/>
+      <c r="AC29" s="6"/>
+      <c r="AD29" s="6"/>
+    </row>
+    <row r="30" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="34"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="42"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M30" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="N30" s="22"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="6"/>
+    </row>
+    <row r="31" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A31" s="46"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="6"/>
+      <c r="Z31" s="6"/>
+      <c r="AA31" s="6"/>
+      <c r="AB31" s="6"/>
+      <c r="AC31" s="6"/>
+      <c r="AD31" s="6"/>
+    </row>
+    <row r="32" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="47"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
+      <c r="X32" s="6"/>
+      <c r="Y32" s="6"/>
+      <c r="Z32" s="6"/>
+      <c r="AA32" s="6"/>
+      <c r="AB32" s="6"/>
+      <c r="AC32" s="6"/>
+      <c r="AD32" s="6"/>
+    </row>
+    <row r="33" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="47"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="43"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="6"/>
+      <c r="U33" s="6"/>
+      <c r="V33" s="6"/>
+      <c r="W33" s="6"/>
+      <c r="X33" s="6"/>
+      <c r="Y33" s="6"/>
+      <c r="Z33" s="6"/>
+      <c r="AA33" s="6"/>
+      <c r="AB33" s="6"/>
+      <c r="AC33" s="6"/>
+      <c r="AD33" s="6"/>
+    </row>
+    <row r="34" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="47"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="43"/>
+      <c r="P34" s="36"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="6"/>
+      <c r="Z34" s="6"/>
+      <c r="AA34" s="6"/>
+      <c r="AB34" s="6"/>
+      <c r="AC34" s="6"/>
+      <c r="AD34" s="6"/>
+    </row>
+    <row r="35" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="47"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="43"/>
+      <c r="P35" s="36"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="6"/>
+      <c r="U35" s="6"/>
+      <c r="V35" s="6"/>
+      <c r="W35" s="6"/>
+      <c r="X35" s="6"/>
+      <c r="Y35" s="6"/>
+      <c r="Z35" s="6"/>
+      <c r="AA35" s="6"/>
+      <c r="AB35" s="6"/>
+      <c r="AC35" s="6"/>
+      <c r="AD35" s="6"/>
+    </row>
+    <row r="36" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="47"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
+      <c r="U36" s="6"/>
+      <c r="V36" s="6"/>
+      <c r="W36" s="6"/>
+      <c r="X36" s="6"/>
+      <c r="Y36" s="6"/>
+      <c r="Z36" s="6"/>
+      <c r="AA36" s="6"/>
+      <c r="AB36" s="6"/>
+      <c r="AC36" s="6"/>
+      <c r="AD36" s="6"/>
+    </row>
+    <row r="37" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A37" s="46"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="43"/>
+    </row>
+    <row r="38" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="47"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="43"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="43"/>
+      <c r="O38" s="45"/>
+    </row>
+    <row r="39" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="47"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="43"/>
+      <c r="N39" s="43"/>
+      <c r="O39" s="43"/>
+    </row>
+    <row r="40" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="47"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="43"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="43"/>
+    </row>
+    <row r="41" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="47"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="43"/>
+      <c r="O41" s="43"/>
+    </row>
+    <row r="42" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="47"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="43"/>
+      <c r="O42" s="43"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.41" right="0" top="0.28299999999999997" bottom="0" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add gaming layer to corne5x3
</commit_message>
<xml_diff>
--- a/keyboard-configurations/fwk-v1/layout.xlsx
+++ b/keyboard-configurations/fwk-v1/layout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ibrahim\dotFiles\keyboard-configurations\fwk-v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ibrahim\repos\ibrahimmkhalid\dotFiles\keyboard-configurations\fwk-v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF881FF-02E4-44D1-A4B7-1E112AB7F34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4AC8E6-31DA-4CD9-B23B-515C2AD99F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="9" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="183">
   <si>
     <t>,</t>
   </si>
@@ -564,6 +564,12 @@
   </si>
   <si>
     <t>MENU</t>
+  </si>
+  <si>
+    <t>_5</t>
+  </si>
+  <si>
+    <t>&gt;_5</t>
   </si>
 </sst>
 </file>
@@ -1377,7 +1383,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1491,20 +1497,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1865,19 +1857,19 @@
   <dimension ref="A1:AD42"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38:I40"/>
+      <selection activeCell="A37" sqref="A37:O42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="15" width="8.44140625" style="1" customWidth="1"/>
+    <col min="2" max="15" width="8.42578125" style="1" customWidth="1"/>
     <col min="16" max="16" width="9" style="1" customWidth="1"/>
-    <col min="17" max="30" width="8.44140625" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.109375" style="1"/>
+    <col min="17" max="30" width="8.42578125" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>130</v>
       </c>
@@ -1955,7 +1947,7 @@
       </c>
       <c r="AD1" s="32"/>
     </row>
-    <row r="2" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="B2" s="9" t="s">
         <v>30</v>
@@ -2035,7 +2027,7 @@
       </c>
       <c r="AD2" s="13"/>
     </row>
-    <row r="3" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
       <c r="B3" s="9" t="s">
         <v>30</v>
@@ -2115,7 +2107,7 @@
       </c>
       <c r="AD3" s="13"/>
     </row>
-    <row r="4" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="15" t="s">
         <v>30</v>
@@ -2195,7 +2187,7 @@
       </c>
       <c r="AD4" s="20"/>
     </row>
-    <row r="5" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
       <c r="B5" s="3" t="s">
         <v>56</v>
@@ -2239,7 +2231,7 @@
       <c r="AC5" s="4"/>
       <c r="AD5" s="8"/>
     </row>
-    <row r="6" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33"/>
       <c r="B6" s="21"/>
       <c r="C6" s="22"/>
@@ -2279,7 +2271,7 @@
       <c r="AC6" s="22"/>
       <c r="AD6" s="25"/>
     </row>
-    <row r="7" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>132</v>
       </c>
@@ -2357,7 +2349,7 @@
       </c>
       <c r="AD7" s="8"/>
     </row>
-    <row r="8" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="9" t="s">
         <v>30</v>
@@ -2437,7 +2429,7 @@
       </c>
       <c r="AD8" s="26"/>
     </row>
-    <row r="9" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="9" t="s">
         <v>30</v>
@@ -2517,7 +2509,7 @@
       </c>
       <c r="AD9" s="13"/>
     </row>
-    <row r="10" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="33"/>
       <c r="B10" s="15" t="s">
         <v>30</v>
@@ -2597,7 +2589,7 @@
       </c>
       <c r="AD10" s="20"/>
     </row>
-    <row r="11" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
       <c r="B11" s="3" t="s">
         <v>30</v>
@@ -2641,7 +2633,7 @@
       <c r="AC11" s="4"/>
       <c r="AD11" s="8"/>
     </row>
-    <row r="12" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
@@ -2681,7 +2673,7 @@
       <c r="AC12" s="22"/>
       <c r="AD12" s="25"/>
     </row>
-    <row r="13" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>128</v>
       </c>
@@ -2739,7 +2731,7 @@
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
     </row>
-    <row r="14" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="9" t="s">
         <v>30</v>
@@ -2799,7 +2791,7 @@
       <c r="AC14" s="6"/>
       <c r="AD14" s="6"/>
     </row>
-    <row r="15" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="9" t="s">
         <v>30</v>
@@ -2859,7 +2851,7 @@
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
     </row>
-    <row r="16" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="15" t="s">
         <v>30</v>
@@ -2919,7 +2911,7 @@
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
     </row>
-    <row r="17" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="33"/>
       <c r="B17" s="3" t="s">
         <v>56</v>
@@ -2963,7 +2955,7 @@
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
     </row>
-    <row r="18" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
@@ -3003,7 +2995,7 @@
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
     </row>
-    <row r="19" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>129</v>
       </c>
@@ -3061,7 +3053,7 @@
       <c r="AC19" s="6"/>
       <c r="AD19" s="6"/>
     </row>
-    <row r="20" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
       <c r="B20" s="9" t="s">
         <v>30</v>
@@ -3121,7 +3113,7 @@
       <c r="AC20" s="6"/>
       <c r="AD20" s="6"/>
     </row>
-    <row r="21" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="33"/>
       <c r="B21" s="9" t="s">
         <v>30</v>
@@ -3181,7 +3173,7 @@
       <c r="AC21" s="6"/>
       <c r="AD21" s="6"/>
     </row>
-    <row r="22" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="33"/>
       <c r="B22" s="15" t="s">
         <v>30</v>
@@ -3241,7 +3233,7 @@
       <c r="AC22" s="6"/>
       <c r="AD22" s="6"/>
     </row>
-    <row r="23" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
       <c r="B23" s="3" t="s">
         <v>56</v>
@@ -3285,7 +3277,7 @@
       <c r="AC23" s="6"/>
       <c r="AD23" s="6"/>
     </row>
-    <row r="24" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="33"/>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
@@ -3325,7 +3317,7 @@
       <c r="AC24" s="6"/>
       <c r="AD24" s="6"/>
     </row>
-    <row r="25" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>154</v>
       </c>
@@ -3383,7 +3375,7 @@
       <c r="AC25" s="6"/>
       <c r="AD25" s="6"/>
     </row>
-    <row r="26" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
       <c r="B26" s="9" t="s">
         <v>30</v>
@@ -3443,7 +3435,7 @@
       <c r="AC26" s="6"/>
       <c r="AD26" s="6"/>
     </row>
-    <row r="27" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="33"/>
       <c r="B27" s="9" t="s">
         <v>30</v>
@@ -3503,7 +3495,7 @@
       <c r="AC27" s="6"/>
       <c r="AD27" s="6"/>
     </row>
-    <row r="28" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="33"/>
       <c r="B28" s="15" t="s">
         <v>30</v>
@@ -3563,7 +3555,7 @@
       <c r="AC28" s="6"/>
       <c r="AD28" s="6"/>
     </row>
-    <row r="29" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="33"/>
       <c r="B29" s="3" t="s">
         <v>56</v>
@@ -3607,7 +3599,7 @@
       <c r="AC29" s="6"/>
       <c r="AD29" s="6"/>
     </row>
-    <row r="30" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="34"/>
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
@@ -3647,7 +3639,7 @@
       <c r="AC30" s="6"/>
       <c r="AD30" s="6"/>
     </row>
-    <row r="31" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>143</v>
       </c>
@@ -3705,7 +3697,7 @@
       <c r="AC31" s="6"/>
       <c r="AD31" s="6"/>
     </row>
-    <row r="32" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="33"/>
       <c r="B32" s="9" t="s">
         <v>30</v>
@@ -3765,7 +3757,7 @@
       <c r="AC32" s="6"/>
       <c r="AD32" s="6"/>
     </row>
-    <row r="33" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="33"/>
       <c r="B33" s="9" t="s">
         <v>30</v>
@@ -3825,7 +3817,7 @@
       <c r="AC33" s="6"/>
       <c r="AD33" s="6"/>
     </row>
-    <row r="34" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="33"/>
       <c r="B34" s="15" t="s">
         <v>30</v>
@@ -3885,7 +3877,7 @@
       <c r="AC34" s="6"/>
       <c r="AD34" s="6"/>
     </row>
-    <row r="35" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="33"/>
       <c r="B35" s="3" t="s">
         <v>30</v>
@@ -3931,7 +3923,7 @@
       <c r="AC35" s="6"/>
       <c r="AD35" s="6"/>
     </row>
-    <row r="36" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="34"/>
       <c r="B36" s="21"/>
       <c r="C36" s="22"/>
@@ -3973,7 +3965,7 @@
       <c r="AC36" s="6"/>
       <c r="AD36" s="6"/>
     </row>
-    <row r="37" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>131</v>
       </c>
@@ -4016,7 +4008,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="33"/>
       <c r="B38" s="9" t="s">
         <v>58</v>
@@ -4061,7 +4053,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="33"/>
       <c r="B39" s="9" t="s">
         <v>60</v>
@@ -4106,7 +4098,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="33"/>
       <c r="B40" s="15" t="s">
         <v>47</v>
@@ -4151,7 +4143,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="33"/>
       <c r="B41" s="3" t="s">
         <v>56</v>
@@ -4180,7 +4172,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="38"/>
       <c r="B42" s="21"/>
       <c r="C42" s="22"/>
@@ -4213,22 +4205,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C4DEAC-AE2C-4CD8-9CB8-A21BA41D0651}">
-  <dimension ref="A1:AE42"/>
+  <dimension ref="A1:AD42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="15" width="8.44140625" style="1" customWidth="1"/>
+    <col min="2" max="15" width="8.42578125" style="1" customWidth="1"/>
     <col min="16" max="16" width="9" style="1" customWidth="1"/>
-    <col min="17" max="30" width="8.44140625" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.109375" style="1"/>
+    <col min="17" max="30" width="8.42578125" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>164</v>
       </c>
@@ -4271,23 +4263,22 @@
         <v>30</v>
       </c>
       <c r="P1" s="2"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="44"/>
-    </row>
-    <row r="2" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+    </row>
+    <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="B2" s="9" t="s">
         <v>30</v>
@@ -4332,23 +4323,22 @@
         <v>30</v>
       </c>
       <c r="P2" s="33"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="44"/>
-    </row>
-    <row r="3" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+    </row>
+    <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
       <c r="B3" s="9" t="s">
         <v>30</v>
@@ -4393,23 +4383,22 @@
         <v>30</v>
       </c>
       <c r="P3" s="33"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="43"/>
-      <c r="AA3" s="43"/>
-      <c r="AB3" s="43"/>
-      <c r="AC3" s="43"/>
-      <c r="AD3" s="43"/>
-      <c r="AE3" s="44"/>
-    </row>
-    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+    </row>
+    <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="15" t="s">
         <v>30</v>
@@ -4454,23 +4443,22 @@
         <v>30</v>
       </c>
       <c r="P4" s="33"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="43"/>
-      <c r="AE4" s="44"/>
-    </row>
-    <row r="5" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+    </row>
+    <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
       <c r="B5" s="3" t="s">
         <v>56</v>
@@ -4499,23 +4487,22 @@
         <v>59</v>
       </c>
       <c r="P5" s="33"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="43"/>
-      <c r="Z5" s="43"/>
-      <c r="AA5" s="43"/>
-      <c r="AB5" s="43"/>
-      <c r="AC5" s="43"/>
-      <c r="AD5" s="43"/>
-      <c r="AE5" s="44"/>
-    </row>
-    <row r="6" spans="1:31" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+    </row>
+    <row r="6" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33"/>
       <c r="B6" s="21"/>
       <c r="C6" s="22"/>
@@ -4540,23 +4527,22 @@
       <c r="N6" s="22"/>
       <c r="O6" s="25"/>
       <c r="P6" s="33"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
-      <c r="U6" s="43"/>
-      <c r="V6" s="43"/>
-      <c r="W6" s="43"/>
-      <c r="X6" s="43"/>
-      <c r="Y6" s="43"/>
-      <c r="Z6" s="43"/>
-      <c r="AA6" s="43"/>
-      <c r="AB6" s="43"/>
-      <c r="AC6" s="43"/>
-      <c r="AD6" s="43"/>
-      <c r="AE6" s="44"/>
-    </row>
-    <row r="7" spans="1:31" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+    </row>
+    <row r="7" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>160</v>
       </c>
@@ -4599,23 +4585,22 @@
         <v>30</v>
       </c>
       <c r="P7" s="40"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="43"/>
-      <c r="S7" s="43"/>
-      <c r="T7" s="43"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="43"/>
-      <c r="X7" s="43"/>
-      <c r="Y7" s="43"/>
-      <c r="Z7" s="43"/>
-      <c r="AA7" s="43"/>
-      <c r="AB7" s="43"/>
-      <c r="AC7" s="43"/>
-      <c r="AD7" s="43"/>
-      <c r="AE7" s="44"/>
-    </row>
-    <row r="8" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+    </row>
+    <row r="8" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="9" t="s">
         <v>30</v>
@@ -4660,23 +4645,22 @@
         <v>30</v>
       </c>
       <c r="P8" s="33"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="43"/>
-      <c r="U8" s="43"/>
-      <c r="V8" s="43"/>
-      <c r="W8" s="43"/>
-      <c r="X8" s="43"/>
-      <c r="Y8" s="43"/>
-      <c r="Z8" s="43"/>
-      <c r="AA8" s="43"/>
-      <c r="AB8" s="43"/>
-      <c r="AC8" s="43"/>
-      <c r="AD8" s="45"/>
-      <c r="AE8" s="44"/>
-    </row>
-    <row r="9" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="37"/>
+    </row>
+    <row r="9" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="9" t="s">
         <v>30</v>
@@ -4721,23 +4705,22 @@
         <v>30</v>
       </c>
       <c r="P9" s="33"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43"/>
-      <c r="V9" s="43"/>
-      <c r="W9" s="43"/>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="43"/>
-      <c r="Z9" s="43"/>
-      <c r="AA9" s="43"/>
-      <c r="AB9" s="43"/>
-      <c r="AC9" s="43"/>
-      <c r="AD9" s="43"/>
-      <c r="AE9" s="44"/>
-    </row>
-    <row r="10" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="33"/>
       <c r="B10" s="15" t="s">
         <v>30</v>
@@ -4782,23 +4765,22 @@
         <v>30</v>
       </c>
       <c r="P10" s="33"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="43"/>
-      <c r="U10" s="43"/>
-      <c r="V10" s="43"/>
-      <c r="W10" s="43"/>
-      <c r="X10" s="43"/>
-      <c r="Y10" s="43"/>
-      <c r="Z10" s="43"/>
-      <c r="AA10" s="43"/>
-      <c r="AB10" s="43"/>
-      <c r="AC10" s="43"/>
-      <c r="AD10" s="43"/>
-      <c r="AE10" s="44"/>
-    </row>
-    <row r="11" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+    </row>
+    <row r="11" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
       <c r="B11" s="3" t="s">
         <v>30</v>
@@ -4827,23 +4809,22 @@
         <v>168</v>
       </c>
       <c r="P11" s="33"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="43"/>
-      <c r="S11" s="43"/>
-      <c r="T11" s="43"/>
-      <c r="U11" s="43"/>
-      <c r="V11" s="43"/>
-      <c r="W11" s="43"/>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="43"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="43"/>
-      <c r="AC11" s="43"/>
-      <c r="AD11" s="43"/>
-      <c r="AE11" s="44"/>
-    </row>
-    <row r="12" spans="1:31" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+    </row>
+    <row r="12" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
@@ -4868,23 +4849,22 @@
       <c r="N12" s="22"/>
       <c r="O12" s="25"/>
       <c r="P12" s="33"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="43"/>
-      <c r="S12" s="43"/>
-      <c r="T12" s="43"/>
-      <c r="U12" s="43"/>
-      <c r="V12" s="43"/>
-      <c r="W12" s="43"/>
-      <c r="X12" s="43"/>
-      <c r="Y12" s="43"/>
-      <c r="Z12" s="43"/>
-      <c r="AA12" s="43"/>
-      <c r="AB12" s="43"/>
-      <c r="AC12" s="43"/>
-      <c r="AD12" s="43"/>
-      <c r="AE12" s="44"/>
-    </row>
-    <row r="13" spans="1:31" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+    </row>
+    <row r="13" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>165</v>
       </c>
@@ -4927,23 +4907,22 @@
         <v>30</v>
       </c>
       <c r="P13" s="35"/>
-      <c r="Q13" s="43"/>
-      <c r="R13" s="43"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-      <c r="U13" s="43"/>
-      <c r="V13" s="43"/>
-      <c r="W13" s="43"/>
-      <c r="X13" s="43"/>
-      <c r="Y13" s="43"/>
-      <c r="Z13" s="43"/>
-      <c r="AA13" s="43"/>
-      <c r="AB13" s="43"/>
-      <c r="AC13" s="43"/>
-      <c r="AD13" s="43"/>
-      <c r="AE13" s="44"/>
-    </row>
-    <row r="14" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
+    </row>
+    <row r="14" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="9" t="s">
         <v>30</v>
@@ -5003,7 +4982,7 @@
       <c r="AC14" s="6"/>
       <c r="AD14" s="6"/>
     </row>
-    <row r="15" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="9" t="s">
         <v>30</v>
@@ -5063,7 +5042,7 @@
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
     </row>
-    <row r="16" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="15" t="s">
         <v>30</v>
@@ -5123,7 +5102,7 @@
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
     </row>
-    <row r="17" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="33"/>
       <c r="B17" s="3" t="s">
         <v>56</v>
@@ -5167,7 +5146,7 @@
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
     </row>
-    <row r="18" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
@@ -5207,7 +5186,7 @@
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
     </row>
-    <row r="19" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>169</v>
       </c>
@@ -5265,7 +5244,7 @@
       <c r="AC19" s="6"/>
       <c r="AD19" s="6"/>
     </row>
-    <row r="20" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
       <c r="B20" s="9" t="s">
         <v>30</v>
@@ -5325,7 +5304,7 @@
       <c r="AC20" s="6"/>
       <c r="AD20" s="6"/>
     </row>
-    <row r="21" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="33"/>
       <c r="B21" s="9" t="s">
         <v>30</v>
@@ -5385,7 +5364,7 @@
       <c r="AC21" s="6"/>
       <c r="AD21" s="6"/>
     </row>
-    <row r="22" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="33"/>
       <c r="B22" s="15" t="s">
         <v>30</v>
@@ -5445,7 +5424,7 @@
       <c r="AC22" s="6"/>
       <c r="AD22" s="6"/>
     </row>
-    <row r="23" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
       <c r="B23" s="3" t="s">
         <v>56</v>
@@ -5489,7 +5468,7 @@
       <c r="AC23" s="6"/>
       <c r="AD23" s="6"/>
     </row>
-    <row r="24" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="33"/>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
@@ -5529,7 +5508,7 @@
       <c r="AC24" s="6"/>
       <c r="AD24" s="6"/>
     </row>
-    <row r="25" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>170</v>
       </c>
@@ -5569,7 +5548,7 @@
         <v>30</v>
       </c>
       <c r="O25" s="32" t="s">
-        <v>30</v>
+        <v>182</v>
       </c>
       <c r="P25" s="35"/>
       <c r="Q25" s="6"/>
@@ -5587,21 +5566,21 @@
       <c r="AC25" s="6"/>
       <c r="AD25" s="6"/>
     </row>
-    <row r="26" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
       <c r="B26" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D26" s="43" t="s">
+      <c r="D26" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F26" s="43" t="s">
+      <c r="F26" s="6" t="s">
         <v>108</v>
       </c>
       <c r="G26" s="10" t="s">
@@ -5616,16 +5595,16 @@
       <c r="J26" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K26" s="43" t="s">
+      <c r="K26" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="L26" s="43" t="s">
+      <c r="L26" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M26" s="43" t="s">
+      <c r="M26" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="N26" s="43" t="s">
+      <c r="N26" s="6" t="s">
         <v>30</v>
       </c>
       <c r="O26" s="13" t="s">
@@ -5647,21 +5626,21 @@
       <c r="AC26" s="6"/>
       <c r="AD26" s="6"/>
     </row>
-    <row r="27" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="33"/>
       <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="43" t="s">
+      <c r="C27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F27" s="43" t="s">
+      <c r="F27" s="6" t="s">
         <v>126</v>
       </c>
       <c r="G27" s="10" t="s">
@@ -5676,16 +5655,16 @@
       <c r="J27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K27" s="43" t="s">
+      <c r="K27" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L27" s="43" t="s">
+      <c r="L27" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="M27" s="43" t="s">
+      <c r="M27" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="N27" s="43" t="s">
+      <c r="N27" s="6" t="s">
         <v>30</v>
       </c>
       <c r="O27" s="13" t="s">
@@ -5707,7 +5686,7 @@
       <c r="AC27" s="6"/>
       <c r="AD27" s="6"/>
     </row>
-    <row r="28" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="33"/>
       <c r="B28" s="15" t="s">
         <v>30</v>
@@ -5767,7 +5746,7 @@
       <c r="AC28" s="6"/>
       <c r="AD28" s="6"/>
     </row>
-    <row r="29" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="33"/>
       <c r="B29" s="3" t="s">
         <v>30</v>
@@ -5779,12 +5758,12 @@
         <v>30</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
       <c r="L29" s="7"/>
       <c r="M29" s="4" t="s">
         <v>30</v>
@@ -5811,7 +5790,7 @@
       <c r="AC29" s="6"/>
       <c r="AD29" s="6"/>
     </row>
-    <row r="30" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="34"/>
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
@@ -5851,22 +5830,48 @@
       <c r="AC30" s="6"/>
       <c r="AD30" s="6"/>
     </row>
-    <row r="31" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
+    <row r="31" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1</v>
+      </c>
+      <c r="D31" s="4">
+        <v>2</v>
+      </c>
+      <c r="E31" s="4">
+        <v>3</v>
+      </c>
+      <c r="F31" s="4">
+        <v>4</v>
+      </c>
+      <c r="G31" s="5">
+        <v>5</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="7">
+        <v>6</v>
+      </c>
+      <c r="K31" s="4">
+        <v>7</v>
+      </c>
+      <c r="L31" s="4">
+        <v>8</v>
+      </c>
+      <c r="M31" s="4">
+        <v>9</v>
+      </c>
+      <c r="N31" s="4">
+        <v>0</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="P31" s="35"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
@@ -5883,22 +5888,50 @@
       <c r="AC31" s="6"/>
       <c r="AD31" s="6"/>
     </row>
-    <row r="32" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="47"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="45"/>
+    <row r="32" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O32" s="26" t="s">
+        <v>69</v>
+      </c>
       <c r="P32" s="36"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
@@ -5915,22 +5948,50 @@
       <c r="AC32" s="6"/>
       <c r="AD32" s="6"/>
     </row>
-    <row r="33" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="47"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="43"/>
+    <row r="33" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33"/>
+      <c r="B33" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="O33" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="P33" s="36"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
@@ -5947,22 +6008,50 @@
       <c r="AC33" s="6"/>
       <c r="AD33" s="6"/>
     </row>
-    <row r="34" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="47"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="43"/>
+    <row r="34" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
+      <c r="B34" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="L34" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="M34" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="N34" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="O34" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="P34" s="36"/>
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
@@ -5979,22 +6068,34 @@
       <c r="AC34" s="6"/>
       <c r="AD34" s="6"/>
     </row>
-    <row r="35" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="47"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
+    <row r="35" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
+      <c r="B35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="P35" s="36"/>
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
@@ -6011,22 +6112,30 @@
       <c r="AC35" s="6"/>
       <c r="AD35" s="6"/>
     </row>
-    <row r="36" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="47"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="43"/>
-      <c r="N36" s="43"/>
-      <c r="O36" s="43"/>
+    <row r="36" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="38"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="M36" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="N36" s="22"/>
+      <c r="O36" s="25"/>
       <c r="P36" s="36"/>
       <c r="Q36" s="6"/>
       <c r="R36" s="6"/>
@@ -6043,107 +6152,107 @@
       <c r="AC36" s="6"/>
       <c r="AD36" s="6"/>
     </row>
-    <row r="37" spans="1:30" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="43"/>
-      <c r="N37" s="43"/>
-      <c r="O37" s="43"/>
-    </row>
-    <row r="38" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="47"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="43"/>
-      <c r="M38" s="43"/>
-      <c r="N38" s="43"/>
-      <c r="O38" s="45"/>
-    </row>
-    <row r="39" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="47"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="43"/>
-      <c r="L39" s="43"/>
-      <c r="M39" s="43"/>
-      <c r="N39" s="43"/>
-      <c r="O39" s="43"/>
-    </row>
-    <row r="40" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="47"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="43"/>
-      <c r="M40" s="43"/>
-      <c r="N40" s="43"/>
-      <c r="O40" s="43"/>
-    </row>
-    <row r="41" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="47"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43"/>
-      <c r="M41" s="43"/>
-      <c r="N41" s="43"/>
-      <c r="O41" s="43"/>
-    </row>
-    <row r="42" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="47"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
-      <c r="K42" s="43"/>
-      <c r="L42" s="43"/>
-      <c r="M42" s="43"/>
-      <c r="N42" s="43"/>
-      <c r="O42" s="43"/>
+    <row r="37" spans="1:30" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="35"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+    </row>
+    <row r="38" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="36"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="37"/>
+    </row>
+    <row r="39" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="36"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="36"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+    </row>
+    <row r="41" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="36"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+    </row>
+    <row r="42" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="36"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.41" right="0" top="0.28299999999999997" bottom="0" header="0" footer="0"/>

</xml_diff>